<commit_message>
Updated Template and Info files
see issue #11 @ International-Soil-Radiocarbon-Database/ISRaD
</commit_message>
<xml_diff>
--- a/inst/extdata/ISRaD_Template_Info.xlsx
+++ b/inst/extdata/ISRaD_Template_Info.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greymonroe/github/ISRaD/inst/extdata/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7DD3A3-B47C-1748-B734-C21A7436F679}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="460" windowWidth="30600" windowHeight="18840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="460" windowWidth="30600" windowHeight="18840" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="general info" sheetId="6" r:id="rId1"/>
@@ -23,13 +17,13 @@
     <sheet name="fraction" sheetId="5" r:id="rId8"/>
     <sheet name="incubation" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -986,7 +980,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="134"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">, which is a linked list of </t>
@@ -1008,7 +1002,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="134"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">(or tabs) descibing a dataset. Synthesis datasets may be entered as a single template but will be automatically partioned into discrete entries based on the original data sources compiled for the synthesis. </t>
@@ -2662,14 +2656,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2787,6 +2781,11 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri (Body)_x0000_"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -3110,7 +3109,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3240,6 +3239,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="290">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3867,14 +3867,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.6640625" customWidth="1"/>
     <col min="2" max="2" width="117.6640625" customWidth="1"/>
@@ -3888,7 +3888,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="64">
+    <row r="2" spans="1:2" ht="60">
       <c r="A2" s="5" t="s">
         <v>260</v>
       </c>
@@ -3896,7 +3896,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="48">
+    <row r="3" spans="1:2" ht="30">
       <c r="A3" s="5" t="s">
         <v>310</v>
       </c>
@@ -3904,7 +3904,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="32">
+    <row r="4" spans="1:2" ht="30">
       <c r="A4" s="5" t="s">
         <v>304</v>
       </c>
@@ -3912,7 +3912,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="48">
+    <row r="5" spans="1:2" ht="45">
       <c r="A5" s="5" t="s">
         <v>262</v>
       </c>
@@ -3920,7 +3920,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="160">
+    <row r="6" spans="1:2" ht="150">
       <c r="A6" s="5" t="s">
         <v>261</v>
       </c>
@@ -3928,7 +3928,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="80">
+    <row r="7" spans="1:2" ht="75">
       <c r="A7" s="5" t="s">
         <v>278</v>
       </c>
@@ -3936,7 +3936,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="64">
+    <row r="8" spans="1:2" ht="60">
       <c r="A8" s="5" t="s">
         <v>302</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="80">
+    <row r="9" spans="1:2" ht="75">
       <c r="A9" s="5" t="s">
         <v>303</v>
       </c>
@@ -3994,14 +3994,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.33203125" bestFit="1" customWidth="1"/>
@@ -4030,7 +4030,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30">
+    <row r="2" spans="1:6" ht="28">
       <c r="A2" s="24" t="s">
         <v>365</v>
       </c>
@@ -4050,7 +4050,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30">
+    <row r="3" spans="1:6" ht="28">
       <c r="A3" s="24" t="s">
         <v>370</v>
       </c>
@@ -4068,7 +4068,7 @@
       </c>
       <c r="F3" s="12"/>
     </row>
-    <row r="4" spans="1:6" ht="30">
+    <row r="4" spans="1:6" ht="28">
       <c r="A4" s="24" t="s">
         <v>0</v>
       </c>
@@ -4212,7 +4212,7 @@
       </c>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="1:6" ht="30">
+    <row r="12" spans="1:6" ht="28">
       <c r="A12" s="12" t="s">
         <v>215</v>
       </c>
@@ -4230,7 +4230,7 @@
       </c>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:6" ht="30">
+    <row r="13" spans="1:6">
       <c r="A13" s="26" t="s">
         <v>373</v>
       </c>
@@ -4259,14 +4259,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="37.33203125" style="1" customWidth="1"/>
@@ -4305,7 +4305,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30">
+    <row r="2" spans="1:9" ht="28">
       <c r="A2" s="24" t="s">
         <v>365</v>
       </c>
@@ -4430,7 +4430,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="30">
+    <row r="7" spans="1:9" ht="28">
       <c r="A7" s="11" t="s">
         <v>380</v>
       </c>
@@ -4456,7 +4456,7 @@
         <v>8900</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30">
+    <row r="8" spans="1:9" ht="28">
       <c r="A8" s="11" t="s">
         <v>28</v>
       </c>
@@ -4493,14 +4493,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="107" zoomScaleNormal="70" zoomScalePageLayoutView="119" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="107" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="31.1640625" style="1" customWidth="1"/>
@@ -4541,7 +4541,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30">
+    <row r="2" spans="1:9" ht="28">
       <c r="A2" s="24" t="s">
         <v>365</v>
       </c>
@@ -4610,7 +4610,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30">
+    <row r="5" spans="1:9" ht="28">
       <c r="A5" s="10" t="s">
         <v>393</v>
       </c>
@@ -4703,7 +4703,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="30">
+    <row r="9" spans="1:9" ht="28">
       <c r="A9" s="10" t="s">
         <v>383</v>
       </c>
@@ -4956,7 +4956,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="30">
+    <row r="20" spans="1:9" ht="28">
       <c r="A20" s="11" t="s">
         <v>388</v>
       </c>
@@ -5048,7 +5048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="30">
+    <row r="24" spans="1:9" ht="28">
       <c r="A24" s="14" t="s">
         <v>408</v>
       </c>
@@ -5074,7 +5074,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="30">
+    <row r="25" spans="1:9" ht="28">
       <c r="A25" s="11" t="s">
         <v>409</v>
       </c>
@@ -5094,7 +5094,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="60">
+    <row r="26" spans="1:9" ht="56">
       <c r="A26" s="14" t="s">
         <v>410</v>
       </c>
@@ -5160,7 +5160,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="45">
+    <row r="29" spans="1:9" ht="42">
       <c r="A29" s="11" t="s">
         <v>413</v>
       </c>
@@ -5183,7 +5183,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="30">
+    <row r="30" spans="1:9" ht="28">
       <c r="A30" s="14" t="s">
         <v>414</v>
       </c>
@@ -5206,7 +5206,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="30">
+    <row r="31" spans="1:9" ht="28">
       <c r="A31" s="14" t="s">
         <v>415</v>
       </c>
@@ -5232,7 +5232,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="30">
+    <row r="32" spans="1:9" ht="28">
       <c r="A32" s="14" t="s">
         <v>416</v>
       </c>
@@ -5282,7 +5282,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="45">
+    <row r="34" spans="1:9" ht="42">
       <c r="A34" s="14" t="s">
         <v>418</v>
       </c>
@@ -5331,7 +5331,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="30">
+    <row r="36" spans="1:9" ht="28">
       <c r="A36" s="11" t="s">
         <v>391</v>
       </c>
@@ -5357,7 +5357,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="30">
+    <row r="37" spans="1:9" ht="28">
       <c r="A37" s="11" t="s">
         <v>392</v>
       </c>
@@ -5394,7 +5394,7 @@
     <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5404,14 +5404,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="117" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="117" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" customWidth="1"/>
@@ -5451,7 +5451,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30">
+    <row r="2" spans="1:9" ht="28">
       <c r="A2" s="24" t="s">
         <v>365</v>
       </c>
@@ -5593,7 +5593,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" ht="16">
       <c r="A8" s="27" t="s">
         <v>421</v>
       </c>
@@ -6212,7 +6212,7 @@
     <mergeCell ref="E6:E7"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E27" r:id="rId1" display="Radiocarbon Laboratory ID (look up here)" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="E27" r:id="rId1" display="Radiocarbon Laboratory ID (look up here)"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6225,14 +6225,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I280"/>
   <sheetViews>
-    <sheetView zoomScale="111" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView zoomScale="111" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="19.83203125" style="23" customWidth="1"/>
     <col min="3" max="3" width="34.5" style="23" customWidth="1"/>
@@ -6389,11 +6389,11 @@
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="39" t="s">
         <v>592</v>
       </c>
       <c r="B7" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>593</v>
@@ -6472,7 +6472,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30">
+    <row r="11" spans="1:9" ht="28">
       <c r="A11" s="11" t="s">
         <v>585</v>
       </c>
@@ -6632,7 +6632,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="30">
+    <row r="19" spans="1:8" ht="28">
       <c r="A19" s="11" t="s">
         <v>515</v>
       </c>
@@ -6658,7 +6658,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="30">
+    <row r="20" spans="1:8" ht="28">
       <c r="A20" s="11" t="s">
         <v>516</v>
       </c>
@@ -6684,7 +6684,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="30">
+    <row r="21" spans="1:8" ht="28">
       <c r="A21" s="11" t="s">
         <v>517</v>
       </c>
@@ -7156,7 +7156,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="30">
+    <row r="42" spans="1:8" ht="28">
       <c r="A42" s="11" t="s">
         <v>532</v>
       </c>
@@ -7176,7 +7176,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="30">
+    <row r="43" spans="1:8" ht="28">
       <c r="A43" s="11" t="s">
         <v>533</v>
       </c>
@@ -7222,7 +7222,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="30">
+    <row r="45" spans="1:8" ht="28">
       <c r="A45" s="11" t="s">
         <v>535</v>
       </c>
@@ -7242,7 +7242,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="30">
+    <row r="46" spans="1:8" ht="28">
       <c r="A46" s="11" t="s">
         <v>536</v>
       </c>
@@ -7482,7 +7482,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="30">
+    <row r="56" spans="1:9" ht="28">
       <c r="A56" s="11" t="s">
         <v>545</v>
       </c>
@@ -7502,7 +7502,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="30">
+    <row r="57" spans="1:9" ht="28">
       <c r="A57" s="11" t="s">
         <v>783</v>
       </c>
@@ -7562,7 +7562,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="30">
+    <row r="60" spans="1:9" ht="28">
       <c r="A60" s="11" t="s">
         <v>548</v>
       </c>
@@ -7734,7 +7734,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="30">
+    <row r="68" spans="1:8" ht="28">
       <c r="A68" s="11" t="s">
         <v>554</v>
       </c>
@@ -7852,7 +7852,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="30">
+    <row r="73" spans="1:8" ht="28">
       <c r="A73" s="11" t="s">
         <v>558</v>
       </c>
@@ -7970,7 +7970,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="30">
+    <row r="78" spans="1:8" ht="28">
       <c r="A78" s="11" t="s">
         <v>563</v>
       </c>
@@ -8070,7 +8070,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="30">
+    <row r="82" spans="1:9" ht="28">
       <c r="A82" s="11" t="s">
         <v>567</v>
       </c>
@@ -8395,7 +8395,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="30">
+    <row r="94" spans="1:9" ht="28">
       <c r="A94" s="11" t="s">
         <v>578</v>
       </c>
@@ -9817,14 +9817,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16385"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="200" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="200" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23.1640625" style="34" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.1640625" style="34" customWidth="1"/>
@@ -9866,7 +9866,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="2" spans="1:9" customFormat="1" ht="45">
+    <row r="2" spans="1:9" customFormat="1" ht="42">
       <c r="A2" s="24" t="s">
         <v>365</v>
       </c>
@@ -75889,14 +75889,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I349"/>
   <sheetViews>
-    <sheetView topLeftCell="D8" zoomScale="114" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="D8" zoomScale="114" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="44" customWidth="1"/>
@@ -75938,7 +75938,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="2" spans="1:9" customFormat="1" ht="30">
+    <row r="2" spans="1:9" customFormat="1" ht="28">
       <c r="A2" s="24" t="s">
         <v>365</v>
       </c>
@@ -76050,7 +76050,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="17" customFormat="1" ht="30">
+    <row r="7" spans="1:9" s="17" customFormat="1" ht="28">
       <c r="A7" s="10" t="s">
         <v>762</v>
       </c>
@@ -76070,7 +76070,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="17" customFormat="1" ht="30">
+    <row r="8" spans="1:9" s="17" customFormat="1" ht="28">
       <c r="A8" s="11" t="s">
         <v>764</v>
       </c>
@@ -76407,7 +76407,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="17" customFormat="1" ht="30">
+    <row r="23" spans="1:8" s="17" customFormat="1" ht="28">
       <c r="A23" s="11" t="s">
         <v>729</v>
       </c>
@@ -76433,7 +76433,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="17" customFormat="1" ht="28">
+    <row r="24" spans="1:8" s="17" customFormat="1">
       <c r="A24" s="11" t="s">
         <v>732</v>
       </c>
@@ -76459,7 +76459,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="17" customFormat="1" ht="30">
+    <row r="25" spans="1:8" s="17" customFormat="1" ht="28">
       <c r="A25" s="11" t="s">
         <v>733</v>
       </c>
@@ -76729,7 +76729,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="17" customFormat="1" ht="30">
+    <row r="37" spans="1:9" s="17" customFormat="1" ht="28">
       <c r="A37" s="11" t="s">
         <v>847</v>
       </c>
@@ -76768,7 +76768,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="17" customFormat="1" ht="30">
+    <row r="39" spans="1:9" s="17" customFormat="1" ht="28">
       <c r="A39" s="11" t="s">
         <v>849</v>
       </c>
@@ -77002,7 +77002,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="49" spans="1:9" s="17" customFormat="1" ht="30">
+    <row r="49" spans="1:9" s="17" customFormat="1" ht="28">
       <c r="A49" s="11" t="s">
         <v>794</v>
       </c>
@@ -77120,7 +77120,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="54" spans="1:9" s="17" customFormat="1" ht="30">
+    <row r="54" spans="1:9" s="17" customFormat="1" ht="28">
       <c r="A54" s="11" t="s">
         <v>799</v>
       </c>
@@ -78473,14 +78473,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" zoomScale="111" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="111" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.1640625" style="42" customWidth="1"/>
@@ -78520,7 +78520,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45">
+    <row r="2" spans="1:9" ht="42">
       <c r="A2" s="24" t="s">
         <v>365</v>
       </c>
@@ -78613,11 +78613,11 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="59" t="s">
         <v>584</v>
       </c>
-      <c r="B6" s="42" t="s">
-        <v>811</v>
+      <c r="B6" s="40" t="s">
+        <v>812</v>
       </c>
       <c r="C6" t="s">
         <v>679</v>

</xml_diff>